<commit_message>
Atouts humains au complet
</commit_message>
<xml_diff>
--- a/Atouts.xlsx
+++ b/Atouts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bertolen\Documents\JdR\Univers\Chroniques des Ténèbres\Ferae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD69A535-281D-49C0-AC09-499E72B77FA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ABE8A8-201F-4C66-B6BA-A7C28C23DBA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,13 +16,15 @@
     <sheet name="Mentaux" sheetId="1" r:id="rId1"/>
     <sheet name="Physique" sheetId="2" r:id="rId2"/>
     <sheet name="Sociaux" sheetId="4" r:id="rId3"/>
-    <sheet name="Surnaturels" sheetId="5" r:id="rId4"/>
-    <sheet name="Combat" sheetId="6" r:id="rId5"/>
+    <sheet name="Surnaturel (humain)" sheetId="7" r:id="rId4"/>
+    <sheet name="Combat" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Combat!$A$1:$D$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mentaux!$A$1:$E$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Physique!$B$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sociaux!$B$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Surnaturel (humain)'!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="175">
   <si>
     <t>Nom</t>
   </si>
@@ -447,6 +449,337 @@
   <si>
     <t>True Friend (•••)
 Effect: Your character has a true friend. While that friend may have specific functions covered by other Merits (Allies, Contacts, Retainer, Mentor, et cetera), True Friend represents a deeper, truly trusting relationship that cannot be breached. Unless your character does something egregious to cause it, her True Friend will not betray her. The Storyteller cannot kill a True Friend as part of a plot without your express permission. Any rolls to influence a True Friend against your character suffer a five-die penalty. In addition, once per story your character can regain one spent Willpower by having a meaningful interaction with her True Friend.</t>
+  </si>
+  <si>
+    <t>Aura Reading</t>
+  </si>
+  <si>
+    <t>•••</t>
+  </si>
+  <si>
+    <t>Your character has the psychic ability to perceive auras; the ephemeral halos of energy that surround all living things. This allows her to perceive a subject’s emotional state, and potentially any supernatural nature. The colors of an aura show a person’s general disposition, and the ebbs, flows, tone, and other oddities reveal other influences. Note that your character may not know what she’s looking at when seeing something odd in an aura. For example, she may not know that a pale aura means she’s seeing a vampire, unless she’s confirmed other vampiric auras in the past.
+To activate Aura Reading, spend a point of Willpower and roll Wits + Empathy – the subject’s Composure. Perceiving an aura takes an uninterrupted moment of staring, which could look suspicious even to the unaware. For every success, ask the subject’s player one of the following questions. Alternatively, take +1 on Social rolls against the character during the same scene, due to the understanding of their emotional state.
+• What’s your character’s most prominent emotion?
+• Is your character telling the truth?
+• What is your character’s attention most focused on right now?
+• Is your character going to attack?
+• What emotion is your character trying most to hide?
+• Is your character supernatural or otherwise not human?
+Determine how your character perceives auras. Maybe she sees different hues as different emotions. Perhaps she hears whispers in the back of her mind, reflecting subtle truths in her subject.</t>
+  </si>
+  <si>
+    <t>Because of your character’s sensitivity to the supernatural, she sometimes appears to know “a little too much.” No more than once per chapter, when first meeting a supernatural creature the Storyteller can roll Wits + Occult for the creature, penalized by your character’s Composure. If successful, they get a strange feeling that your character is aware of their nature. They’re not forced to behave in any particular way, but it could cause complications.</t>
+  </si>
+  <si>
+    <t>Biokinesis</t>
+  </si>
+  <si>
+    <t>Your character has the ability to psychically alter her biological material. By spending a Willpower point and concentrating for a full minute, she can shift her Physical Attributes. She can shift one dot per dot in this Merit. This shift lasts for one hour. This cannot raise an Attribute higher than five dots.
+In addition, the character heals quickly. Halve all healing times.</t>
+  </si>
+  <si>
+    <t>Clairvoyance</t>
+  </si>
+  <si>
+    <t>Your character can project her senses to another location. She sees, hears, smells, and otherwise experiences the other place as if she were there. This ability requires a point of Willpower to activate, successful meditation, and a Wits + Occult roll. Suggested Modifiers: Has an object important to the place (+1), never been there (–3), scrying for a person and not a place (–3), scrying for non-specific location (–4), spent significant time there (+2), touching someone with a strong connection to the place (+1)</t>
+  </si>
+  <si>
+    <t>When choosing this ability, determine how your character is able to scry. It may be through a crystal ball, through a drug-induced trance, with esoteric computer models, or any other method. She cannot scry without that tool or methodology.</t>
+  </si>
+  <si>
+    <t>Cursed</t>
+  </si>
+  <si>
+    <t>Your character has run afoul of fate. Somewhere, somehow, she’s been cursed. Most importantly, she’s aware of the curse. When taking this Merit, define the limitations of the curse. Usually, it’s expressed in the form of a single statement, such as, “On the eve of your twenty-seventh birthday, you will feast upon your doom.” It’s important to work out the details with the Storyteller. The curse must take effect within the scope of the planned chronicle.
+While she knows how she’ll die, this is actually a liberating experience. She’s confident of the method of her death so nothing else fazes her. Gain a +2 on any Resolve + Composure roll to face fear or self-doubt. Any time she takes lethal damage in her last three health boxes, take an additional Beat.</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Empathy ••</t>
+  </si>
+  <si>
+    <t>Your character hears the words and moans of the dead. If she takes the time to parse their words, she can interact with them verbally.
+Your character has more than just a knack for knowing when ephemeral beings are lurking nearby — she can reach out and make contact with them. By conducting a ritual, meditating, or otherwise preparing to commune with the unseen and succeeding at a Wits + Occult roll, she temporarily increases the relevant Condition one step along the progression from nothing to Anchor, Resonance or Infrastructure, to Open, and finally to Controlled (see p. 223 for more on Conditions as they relate to spirits). The effect lasts until she spends a Willpower point, but if an Influence has been used to progress the Condition further, doing so only reduces it by one step.</t>
+  </si>
+  <si>
+    <t>Speaking with ghosts can be a blessing, but your character cannot turn the sense off, any more than she can turn off her hearing. The character hears the words of the dead any time they’re present. Once per game session, usually in a time of extreme stress, the Storyteller may deliver a disturbing message to your character from the other side. You must succeed in a Resolve + Composure roll or gain the Shaken or Spooked Condition.</t>
+  </si>
+  <si>
+    <t>Mind of a Madman</t>
+  </si>
+  <si>
+    <t>Empathy •••</t>
+  </si>
+  <si>
+    <t>Your character gets deep into the skin of problems. If she’s investigating a crime or other phenomenon, she can put herself in the mind of the culprit. This often helps with the case. However, it takes her to a dark place internally.
+Once she’s made the choice to sink into the culprit’s mindset (which usually involves intense meditation or perusal of the culprit’s crimes), she gains 8-again on all rolls to investigate, pursue, and stop the culprit. But once per night, while she sleeps, she dreams about the culprit’s crimes and theoretical future crimes. This is intensely traumatic and it drives her further on the hunt. If she spends the day without pursuing the culprit, make a breaking point roll as if she’d committed the crime herself. She can resist the dreams and the breaking points by avoiding sleep, but she’s subject to normal deprivation effect. Until the culprit’s captured, any of her own breaking point rolls from things she’s done suffer a –1 penalty.</t>
+  </si>
+  <si>
+    <t>Omen Sensitivity</t>
+  </si>
+  <si>
+    <t>Your character sees signs and patterns in everything. From the way the leaves fall to the spray of antifreeze when her radiator pops, to the ratios of circumference on the shell she picked up on the sidewalk: everything has meaning. With some consideration, she can interpret these meanings. This would be far better if she could turn it off. Everything is important. Everything could mean the end of the world, the deaths of her friends, or other tragedies. If she misses an omen, it might be the wrong one.
+Once per game session, you can make a Wits + Occult roll for your character to interpret an omen in her surroundings. For every success, ask the Storyteller a yes/no question about your character’s life, her surroundings, a task at hand, or the world at large. The Storyteller must answer these questions truthfully.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Her ability becomes an obsession. Each time she reads a portent, she gains the Obsession or Spooked Condition. </t>
+  </si>
+  <si>
+    <t>Psychokinesis</t>
+  </si>
+  <si>
+    <t>••• or •••••</t>
+  </si>
+  <si>
+    <t>Your character has a psychic ability to manipulate the forces of the universe. Every type of Psychokinetic is different. For example, your character might have Pyrokinesis, Cryokinesis, or Electrokinesis, the control of fire, cold, or electricity respectively. This is not an exhaustive list. She can intensify, shape, and douse her particular area of ability. With the three-dot version, some of the given force must be present for her to manipulate. With the five-dot version, she can manifest it from nothingness.
+Spend a point of Willpower to activate Psychokinesis and roll Resolve + Occult. Each success allows a degree of manipulation: choose one of the following options below. If you intend to cause harm with the roll, subtract the victim’s Resolve from the Resolve + Occult roll. If characters should be harmed without a direct attack — if they run through a patch of flame for example — the three-dot version of the Merit causes one lethal damage and the five-dot version causes two. The Storyteller may rule that larger manifestations cause more, if the situation calls for it.
+• Increase or decrease the Size of the manifestation by one.
+• Move the manifestation a number of yards equal to your character’s Willpower dots times 2.
+• Shape the force into a specific form. This may require an Intelligence + Crafts roll to form into a detailed or intricate shape.
+• Attack a victim with the force. Allocate any number of the rolled successes to cause harm. With the three-dot Merit, Psychokinesis is a weapon causing 1L damage. Psychokinesis is considered a 2L weapon with the five- dot version.
+• Use the force creatively. This is up to the situation and the force in question. For example, an Electrokinetic may use her ability to power an electronic device briefly or jumpstart a stalled automobile.
+• Manifest her force. This only works with the five-dot version. It manifests a Size 1 patch of the force. It may spread or be enlarged with further successes.</t>
+  </si>
+  <si>
+    <t>Whenever your character depletes her last Willpower point, the Storyteller can call on her abilities to manifest spontaneously. Resist this with a Resolve + Composure roll, with a –2 penalty if her chosen force is prominently featured nearby. For example, the penalty applies if a Pyrokinetic is locked in a factory with a hot forge. This tends to happen during wildly inconvenient moments and in ways that tend to cause more trouble than they solve. With these wild manifestations, use of Psychokinesis does not cost Willpower.</t>
+  </si>
+  <si>
+    <t>Psychometry</t>
+  </si>
+  <si>
+    <t>Psychometry is the psychic ability to read impressions left on physical objects. Your character can feel the emotional resonance left on an item or can perceive important events tied to a location with this ability. The ability automatically hones in on the most emotionally intense moment tied to the item.
+Spend a Willpower point to activate Psychometry. The successes scored on a Wits + Occult roll determine the clarity of the visions. For each success, you may ask a single yes/ no question of the Storyteller, or one of the following questions. For questions pertaining to specific characters, if your character hasn’t met the persons in question, the Storyteller may simply describe them.
+• What’s the strongest emotion here?
+• Who remembers this moment the most?
+• Am I missing something in this scene?
+• Where was this object during the event?
+• What breaking point caused the event?
+Suggested Modifiers: Character has read impressions from this item before (–2), important event happened more than one day ago (–1), more than one week ago (–2), more than one month ago (–3), more than one year ago (–5), item was used in a violent crime (+2), item is only vaguely tied to the event (–2), spirits pertaining to the event are nearby (+3)</t>
+  </si>
+  <si>
+    <t>Once per chapter, the Storyteller can force a Psychometry vision any time an important place is visited or an important item is touched. This doesn’t require a roll or Willpower point to activate. The Storyteller can give any information pertaining to the event in question. The Storyteller can also impose one Condition relevant to the event.</t>
+  </si>
+  <si>
+    <t>Telekinesis</t>
+  </si>
+  <si>
+    <t>Your character has a psychic ability to manipulate the physical world with her mind. This means lifting, pushing, and pulling objects. Fine manipulation is beyond the scope of Telekinesis. By spending a Willpower point, she can activate Telekinesis for the scene. Her dots in this Merit determine her mind’s effective Strength for the purpose of lifting and otherwise influencing her environment.
+A telekinetic can use her abilities to cause harm by lashing out at threats. Each “attack” costs a point of Willpower. The dice pool to attack is Telekinesis + Occult, penalized by the opponent’s Stamina. The attack causes bashing damage. Alternatively, it can be used to grapple, with the Merit dots representing the Strength score of the psychic. Any overpowering maneuvers require additional Willpower points.</t>
+  </si>
+  <si>
+    <t>Any time your character suffers injury or intense stimuli, the Storyteller may call for a Resolve + Composure roll to resist activating Telekinesis at an inopportune time. If the Storyteller calls for this roll and it fails, the character activates Telekinesis in a quick, impressive display of the power. That use of Telekinesis is free. The player can choose to automatically fail the Resolve + Composure roll and take a Beat.</t>
+  </si>
+  <si>
+    <t>Telepathy</t>
+  </si>
+  <si>
+    <t>Your character can hear surface thoughts and read minds. With the five-dot version of this Merit, she can broadcast simple messages to others’ minds. She hears these thoughts as if they were spoken, which means they can sometimes be distracting. She could only hear thoughts at the range she could hear normal conversation, regardless of any ambient noise (so a telepath could hear the thoughts of someone next to her at a loud concert, even though she couldn’t actually hear the subject talk, but could not hear the thoughts of someone a football field away under quiet conditions). Spend a point of Willpower to activate Telepathy and roll Wits + Empathy, minus the subject’s Resolve if the subject is unwilling. If successful, the subject’s player must tell you the foremost thought on the character’s mind. Additional successes allow you to ask the subject’s player additional questions from the following list. The questions can be asked any time within the same scene. With the five-dot version, every success offers a single phrase the subject hears as if your character said it. As before, these phrases can be communicated at any time during the same scene.
+• What does your character want right now?
+• What does your character fear most right now?
+• What is your character hiding?
+• What does your character want mine to do?
+• What does your character know about [relevant topic at hand]?
+• What turns your character on right now?
+• What’s something shameful or embarrassing about your character?</t>
+  </si>
+  <si>
+    <t>Sometimes, your character hears things she probably shouldn’t. Once per chapter, the Storyteller can give your character a message of terrible things to come. Perhaps she overhears the mad internal ramblings of a cultist in a crowd. Maybe she hears a plot to hijack a plane. Maybe, just maybe, she hears the incoherent thoughts of the God-Machine. These heard thoughts never just occur. They always happen when your character has something else, something important, something pressing going on. When this happens, the Storyteller gives you a Condition such as Spooked or Shaken.</t>
+  </si>
+  <si>
+    <t>Thief of Fate</t>
+  </si>
+  <si>
+    <t>Your character is a magnet for fortune and fate. When she’s close to someone, she unintentionally steals their good fortune. If she touches someone, this Merit takes effect unless she spends a point of Willpower to curb the effect for a scene. In the same day, any failures the subject makes are considered dramatic failures. If she’s used this Merit in a given day, she gains four dice any time she spends Willpower to increase a dice pool.</t>
+  </si>
+  <si>
+    <t>Once a victim of this Merit suffers a dramatic failure, he hears your character’s name in the back of his mind. This may inspire scrutiny.</t>
+  </si>
+  <si>
+    <t>Unseen Sense</t>
+  </si>
+  <si>
+    <t>Your character has a “sixth sense” for a type of supernatural creature, chosen when you buy the Merit. For example, you may choose Unseen Sense: Vampires, or Unseen Sense: Fairies. The sense manifests differently for everyone. A character’s hair stands on end, she becomes physically ill, or perhaps she has a cold chill. Regardless, she knows that something isn’t right when she is in the immediate proximity of the appropriate supernatural being. Once per chapter, the player can accept the Spooked Condition (p. 183) in exchange for which the character can pinpoint where the feeling is coming from. If the target is using a power that specifically cloaks its supernatural nature, however, this does not work (though the Condition remains until resolved as usual).
+Note: If the character takes “God-Machine” as the focus for this Merit, that character can also see through Concealment Infrastructure (seeing the gears when no one else can, for instance).</t>
+  </si>
+  <si>
+    <t>Armed Defense (Style)</t>
+  </si>
+  <si>
+    <t>Cheap Shot</t>
+  </si>
+  <si>
+    <t>Your character is a master at the bait and switch. She can look off in an odd direction and prompt her opponent to do the same, or she might step on someone’s toes to distract them. Either way, she fights dirty. Make a Dexterity + Subterfuge roll as a reflexive action. The opponent’s player contests with Wits + Composure. If you score more successes, the opponent loses his Defense for the next turn. Each time a character uses this maneuver in a scene, it levies a cumulative –2 penalty to further uses since the opposition gets used to the tricks.</t>
+  </si>
+  <si>
+    <t>Choke Hold</t>
+  </si>
+  <si>
+    <t>If you can get your hands on someone, it’s over. When grappling, you can use the Choke move.
+• Choke: If you rolled more successes than twice the victim’s Stamina, he’s unconscious for (six – Stamina) minutes. You must first have succeeded at a Hold move. If you don’t score enough successes at first, you can Choke your opponent on future turns and total your successes.</t>
+  </si>
+  <si>
+    <t>Defensive Combat</t>
+  </si>
+  <si>
+    <t>Brawl • or Weaponry •; choose one when this Merit is selected</t>
+  </si>
+  <si>
+    <t>You are training in avoiding damage in combat. Use your Brawl or Weaponry to calculate Defense rather than Athletics. You can learn both versions of this Merit, allowing you to use any of the three Skills to calculate Defense. However, you cannot use Weaponry to calculate Defense unless you actually have a weapon in hand.</t>
+  </si>
+  <si>
+    <t>Fighting Finesse</t>
+  </si>
+  <si>
+    <t>Choose a Specialty in Weaponry or Brawl when you purchase this Merit. Your character’s extensive training in that particular weapon or style has allowed them to benefit more from their alacrity and agility than their strength. You may substitute your character’s Dexterity for her Strength when making rolls with that Specialty.
+This Merit may be purchased multiple times to gain its benefit with multiple Specialties.</t>
+  </si>
+  <si>
+    <t>Firefight (Style)</t>
+  </si>
+  <si>
+    <t>Your character is comfortable with a gun. She’s been trained in stressful situations and knows how to keep herself from being shot while shooting at her opponents. This Style is about moving, strafing, and taking shots when you get them. It’s not a series of precision techniques; it’s using a gun practically in a real-world situation.
+Shoot First (•): In a firefight, the person who gets shot first is usually the loser. Your character has trained herself to fire first in an altercation. If her gun is drawn, add her Firearms score to her Initiative. If she has Quick Draw, she can use Shoot First to draw and fire with increased Initiative in the first turn of combat.
+Suppressive Fire (••): Sometimes, the purpose of a shot is to distract, not necessarily to hit. Your character is trained to fire off a handful of rounds with the intent to startle opponents and force impulse reactions. When using the Covering Fire maneuver (p. 200), her opponents cannot benefit from aiming against her. She can apply her Defense against incoming Firearms attacks in addition to any cover bonuses. As well, her training allows her to use Covering Fire with a semi-automatic weapon.
+Secondary Target (•••): Sometimes shooting an opponent behind cover is all but impossible. A bullet can knock objects off balance, however, or cause ricochets. By using Secondary Target, your character opts to not hit her target but instead strike them with any collateral objects that might be nearby. She causes bashing damage instead of lethal, but ignores all cover penalties to the roll. The weapon’s damage rating does not add to the damage in this case.</t>
+  </si>
+  <si>
+    <t>Grappling (Style)</t>
+  </si>
+  <si>
+    <t>Your character has trained in wrestling or one of many grappling martial arts.
+Sprawl (•): Your character can adjust her weight to defend herself in a grapple. While in a grapple, the character’s opponent cannot apply the Drop Prone or Take Cover moves.
+Takedown (••): Your character can take an opponent to the ground rapidly. With a normal roll, you may choose to render an opponent prone instead of establishing a grapple. You may also choose to cause bashing damage equal to the successes rolled.
+Joint Lock (•••): You use joint locks and immobilizing tactics to limit your opponent’s movement. You can use the Joint Lock move in a grapple. Next turn, your opponent suffers bashing damage equal to your successes. You can use Joint Lock as a lead-in to the Restrain move. In addition, any successful overpowering maneuvers your character uses cause 1L damage in addition to their normal effects.</t>
+  </si>
+  <si>
+    <t>Heavy Weapons (Style)</t>
+  </si>
+  <si>
+    <t>Your character is trained with heavy weapons that require strength, wide range, and follow-through more than direct speed and accuracy. This Style may be used with two-handed weapons such as a claymore, a chainsaw, a pike, or an uprooted street sign.
+Sure Strike (•): Your character doesn’t always hit the hardest or the most frequently, but you guarantee a deadly strike when you do hit. You can reflexively remove three dice from any attack dice pool (to a minimum of zero) to add one to your character’s weapon damage rating for the turn. These dice must be removed after calculating any penalties from the environment or the opponent’s Defense.
+Threat Range (••): Your character’s weapon is immense and keeps opponents at bay. If you opt not to move or Dodge during your turn, any character moving into your character’s proximity suffers 1L damage and a penalty to their Defense equal to your character’s weapon damage rating. This penalty only lasts for one turn. This cannot be used in a turn the character is Dodging.
+Bring the Pain (•••): Your character’s strikes stun and incapacitate as well as causing massive trauma to the body. Sacrifice your character’s Defense to use Bring the Pain. Make a standard attack roll. Any damage you score with Bring the Pain counts as a penalty to all actions the victim takes during their next turn. So, if you cause 4L damage, the opponent is at –4 on their next attack.
+Warding Stance (••••): Your character holds her weapon in such a way as to make attacks much harder. If her weapon’s drawn, spend a point of Willpower reflexively to add her weapon’s damage rating as armor for the turn. This will not protect against firearms.
+Rending (•••••): Your character’s cuts leave crippling, permanent wounds. By spending a Willpower point before making an attack roll, her successful attacks cause one point of aggravated damage in addition to her weapon’s damage rating. This Willpower point does not add to the attack roll.</t>
+  </si>
+  <si>
+    <t>Improvised Weaponr (Style)</t>
+  </si>
+  <si>
+    <t>Most people don’t walk around armed. While someone pulling a knife or a gun can cool a hostile situation down, it can also cause things to boil over — an argument that wouldn’t be more than harsh words suddenly ends up with three people in the morgue. If you’re on the receiving end of someone pulling a knife, it helps to have something in your own hand.
+You’re good at making do with what you’ve got. Sometimes, you’re lucky — if you’re in a bar, you’ve got a lot of glass bottles, maybe a pool cue to play with. But you’ve got something almost like a sixth sense for weaponry and can find one almost anywhere.
+Always Armed (•): You can always get your hands on something dangerous, and you’ve an instinctive understanding of how to put it to good — and deadly — use. At the start of your turn, make a reflexive Wits + Weaponry roll to grab an object suitable for use as a weapon in pretty much any environment. (The player is encouraged to work with the Storyteller to determine an appropriate item — a large, jagged rock in the wilderness, for example, or a heavy glass ashtray with one sharp, broken edge in a dive bar.) Regardless of what you pick up, the weapon has a +0 weapon modifier, −1 initiative penalty, Size 1, Durability 2, and Structure 4. On an exceptional success, increase the weapon modifier and Size by 1, but the initiative penalty increases to −2. Whatever you grab doesn’t suffer the normal −1 penalty for wielding an improvised weapon (see p. 205).
+In Harm’s Way (••): You’ve got a knack for putting your weapon in the way of an oncoming attack, no matter how small or inappropriate for blocking it might be. While wielding an improvised weapon acquired with Always Armed, you can treat the Structure of your weapon as general armor against a single Brawl or Weaponry attack. Any damage you take inflicts an equal amount of damage to the improvised weapon, bypassing Durability. You can use the weapon to attack later in the same turn, but can only use this ability when applying your Defense to an attack.
+Breaking Point (•••): One sure way to win a fight is to hit the other guy so hard that he doesn’t get back up, even if that means losing a weapon in the process. When making an all-out attack with an improvised weapon acquired with Always Armed, you can reduce the weapon’s Structure by any amount down to zero. Every two points of Structure spent in this way adds +1 to the weapon modifier for that one single attack. Declare any Structure loss before making the attack; this Structure is reduced even if the attack does no damage. If the weapon is reduced to zero Structure, it is automatically destroyed after the attack.
+You can use this technique in conjunction with In Harm’s Way, allowing you to parry an attack made on a higher Initiative and then go on the offensive, provided that the weapon wasn’t destroyed.</t>
+  </si>
+  <si>
+    <t>Iron Skin</t>
+  </si>
+  <si>
+    <t>•• or ••••</t>
+  </si>
+  <si>
+    <t>Through rigorous conditioning or extensive scarring, your character has grown resistant to harm. She can shrug off shots that would topple bigger fighters. She knows how to take a strike and can even move into a hit from a weapon to minimize harm. She gains armor against bashing attacks; one point of armor with ••, and two points of armor with ••••. By spending a point of Willpower when hit, she can downgrade lethal damage from a successful attack into bashing. Downgrade one point of lethal damage at ••, two points of lethal with ••••.</t>
+  </si>
+  <si>
+    <t>Light Weapons (Style)</t>
+  </si>
+  <si>
+    <t>Your character is trained with small hand-to-hand weapons that favor finesse over raw power. These maneuvers may only be used with one-handed weapons that have a damage rating of 2 or less.
+Rapidity (•): Your character moves with swiftness to find just the right spot to strike. You can sacrifice your character’s weapon damage rating to add her Weaponry score to her Initiative for the turn. The weapon becomes a 0 damage weapon for the turn.
+Thrust (••): Your character knows when to defend herself and when to move in for the kill. At any time, you can sacrifice points of Defense one-for-one to add to attack pools. This cannot happen if you’ve already used Defense in the same turn. If you use this maneuver, you may not sacrifice your full Defense for any other reason. For example, you cannot use Thrust with an all-out attack.
+Feint (•••): With a flourish to one direction, your character can distract an opponent for a cleaner, more effective follow-up strike. Make an attack roll as normal, but the attack causes no damage. The next attack your character makes against the same opponent ignores Defense equal to the damage the attack would have caused, and adds the feint’s successes rolled as additional damage if successful.
+Flurry (••••): Your character moves quickly enough to stab opponents with numerous pricks and swipes in the blink of an eye. As long as your character has her Defense available to her (it’s not been sacrificed for another maneuver or denied from surprise, for example), any character coming into her immediate proximity takes one point of lethal damage. This damage continues once per turn as long as the enemy stays within range and occurs on the enemy’s turn. This can affect multiple opponents but cannot be used in a turn where the character is Dodging.
+Vital Shot (•••••): Your character can use her smaller weapon to get past an opponent’s defenses and hit where it hurts most. Sacrifice your character’s Defense for the turn to use this maneuver. If the attack roll succeeds, the attack causes one point of aggravated damage in addition to the damage rating of the weapon.</t>
+  </si>
+  <si>
+    <t>Marksmanship (Style)</t>
+  </si>
+  <si>
+    <t>When prepared and aimed, a gun is an ideal killing machine. Your character has trained to take advantage of the greatest features of any gun. This Style is often used with rifles, but it can be used with any type of firearm. Because of the discipline and patience required for Marksmanship, your character cannot use her Defense in any turn in which she uses one of these maneuvers. These maneuvers may only be used after aiming for at least one turn.
+Through the Crosshairs (•): Your character is a competent sniper, able to sit in position and steel her wits. Usually, the maximum bonus from aiming is three dice. With Through the Crosshairs, it’s equal to her Composure + Firearms.
+Precision Shot (••): With this level of training, your character knows how to effectively disable a victim instead of focusing on the kill. When attacking a specified target, you may reduce your weapon’s damage rating one-for-one to ignore penalties for shooting a specified target (see p. 203). For example, if you’re using a sniper rifle (4 damage weapon), and attacking an arm (–2 to hit), you could choose to use 3 damage reduce that to –1, or 2 damage to eliminate the penalty entirely.
+A Shot Rings Out (•••): A master sniper, your character has no worries or lack of confidence. She can fire into a crowd and strike a specific target without penalty. If she misses, it’s because her shot goes wide. She will never hit an unintended target.
+Ghost (••••): Your character has trained to shoot unseen and vanish without a trace. Her Firearms score acts as a penalty on any roll to notice her vantage point, or any Investigation or Perception roll to investigate the area from which she shot.</t>
+  </si>
+  <si>
+    <t>Martial Arts (Style)</t>
+  </si>
+  <si>
+    <t>Your character is trained in one or more formal martial arts styles. This may have come from a personal mentor, a dojo, or a self-defense class. It may have been for exercise, protection, show, or tradition. These maneuvers may only be used unarmed, or with weapons capable of using the Brawl Skill, such as a punch dagger, or a weapon using the Shiv Merit.
+Focused Attack (•): Your character has trained extensively in striking specific parts of an opponent’s body. Reduce penalties for hitting specific targets by one. Additionally, you may ignore one point of armor on any opponent.
+Defensive Strike (••): Your character excels in defending herself while finding the best time to strike. You can add one or two points to your character’s Defense. For each Defense point you take, subtract a die from any attacks you make. This can only be used in a turn in which your character intends to attack. It cannot be used with a Dodge.
+Whirlwind Strike (•••): When engaged, your character becomes a storm of threatening kicks and punches; nothing close is safe. As long as your character has her Defense available to her and is not Dodging, any character coming into arm’s reach takes 1B damage. This damage continues once per turn as long as the enemy stays within range and occurs on the enemy’s turn. If you spend a point of Willpower, this damage becomes 2B until your next turn.
+The Hand as Weapon (••••): With this degree of training, your character’s limbs are hardened to cause massive trauma. Her unarmed strikes cause lethal damage.
+The Touch of Death (•••••): Your character’s mastery has brought with it the daunting power of causing lethal injury with a touch. If she chooses, her unarmed strikes count as weapons with 2 damage rating.</t>
+  </si>
+  <si>
+    <t>Police Tactics (Style)</t>
+  </si>
+  <si>
+    <t>Your character is trained in restraint techniques often used by law enforcement officers. This may reflect formal training or lessons from a skilled practitioner.
+Compliance Hold (•): Once your character has established a Hold in a grapple, your opponent suffers a -3 to all further grappling rolls until your character releases her.
+Weapon Retention (••): Opponents attempting to disarm your character or turn her weapon against her must exceed your character’s Weaponry score in successes.
+Speed Cuff (•••): Against an immobilized opponent, your character may apply handcuffs, cable ties, or similar restraints as a reflexive action.</t>
+  </si>
+  <si>
+    <t>Shiv</t>
+  </si>
+  <si>
+    <t>• or ••</t>
+  </si>
+  <si>
+    <t>Your character carries small, concealable weapons for use in a tussle. Rolls to detect the concealed weapon suffer your character’s Weaponry score as a penalty. With the onedot version, she can conceal a weapon with a 0 damage rating. The two-dot version can conceal a 1 damage rating weapon. Your character may use the Brawl Skill to use this weapon.</t>
+  </si>
+  <si>
+    <t>Street Fighting (Style)</t>
+  </si>
+  <si>
+    <t>Your character learned to fight on the mean streets. She may have had some degree of formal training, but the methodology came from the real world in dangerous circumstances. Street Fighting isn’t about form and grace. It’s about staying alive. These maneuvers may only be used unarmed, with weapons capable of using the Brawl Skill (such as punch daggers), or weapons concealed with the Shiv Merit (above).
+Duck and Weave (•): Your character has been beaten all to hell more than a few times. Now she dodges on instinct, not on skill. You can reflexively take a one-die penalty to any actions this turn in order to use the higher of her Wits and Dexterity to calculate Defense. If you’ve already made a roll without penalty this turn, you cannot use Duck and Weave.
+Knocking the Wind Out (••): Shots to the center mass can shake an opponent, and your character knows this well. When your character makes a successful unarmed attack, the opponent suffers a –1 to his next roll.
+Kick ‘Em While They’re Down (•••): The best enemy is one on the ground. Your character topples opponents and keeps them down. Any time your successes on an attack roll exceed an opponent’s Stamina, you may choose to apply the Knocked Down Tilt (p. 211). Additionally, any time your character is close enough to strike when an opponent attempts to get up from a prone position, she can reflexively cause 2B damage.
+One-Two Punch (••••): Your character hits fast and follows through with every hit. Whenever she makes a successful attack, you can spend a point of Willpower to cause two extra points of bashing damage.
+Last-Ditch Effort (•••••): In a street fight, every second could be the one that kills you. A proficient street fighter is a remarkable survivalist. She bites, headbutts, trips: whatever it takes to prevent that last hit. Any time a character with this level of Street Fighting is about to take a hit or an overpowering maneuver when she’s already suffering wound penalties, she can reflexively spend a Willpower point and sacrifice her Defense for the turn to make an attack against her would-be assailant. This can occur even if she’s already acted in a turn, so long as she’s not already spent Willpower. Resolve this attack before the opponent’s action.</t>
+  </si>
+  <si>
+    <t>Unarmed Defense (Style)</t>
+  </si>
+  <si>
+    <t>You know that hitting someone in the face is an easy way to break the little bones in your hand. To that end, you’ve perfected the art of using the environment to hurt people.
+Firing Lines (•): In some situations, your best option is a tactical retreat — especially if you’ve inadvertently brought a knife to a gunfight. You can run for cover as a reaction to a ranged attack instead of dropping prone (see “Going Prone,” pp. 164–165 of the World of Darkness Rulebook). You give up your action for the turn but can get to any cover that’s within twice your Speed.
+Hard Surfaces (••): Bouncing someone’s head off a urinal, computer monitor, or a brick wall is a handy way to increase the amount of hurt inflicted while not breaking the aforementioned hand bones. When you’re grappling someone, you can bounce them off a hard surface with a Damage move. You deal lethal damage and immediately end the grapple.
+Armored Coffin (•••): The problem with protection is simple: the very things that protect you can be turned against you. That holds true for body armor just as much as anything else. Sure, it blocks bullets and knives, but get in a clinch and you might as well be wearing a straightjacket. When you grapple an opponent, add their general armor rating to your dice pool. When you use a Damage move, ignore your opponent’s armor. This technique can’t be used in conjunction with Hard Surfaces.
+Prep Work (••••): If you’ve got a second to look around, you could catch someone by surprise almost anywhere. When launching a surprise attack, your Dexterity + Stealth roll becomes a rote action.
+Drawback: You can’t use this Merit to set up sniper attacks — your ambush must use Brawl or Weaponry.
+Turnabout (•••••): If you’re caught short in a fight, your opponent’s weapon suits you just fine. When you attempt to Disarm your opponent, step the results up one level — on a failure, your opponent drops the weapon. On a success, you take possession of your opponent’s weapon. On an exceptional success, you’ve got the weapon and your opponent takes two points of bashing damage.</t>
+  </si>
+  <si>
+    <t>You’re better at stopping people from hurting you than you are at hurting other people. Maybe you practice a martial art that redirects an opponent’s blows, or else you’re just very good at not being where your opponent wants you to be.
+Like a Book (•): You can read your opponents and know where they’re likely to strike. When facing an unarmed opponent and not Dodging, increase your Defense by half your Brawl (round down).
+Studied Style (••): You focus on reading one opponent, avoiding his attacks, and frustrating him. Attacks from that opponent do not reduce your Defense. If your Defense reduces his attack pool to 0, his further attacks against you lose the 10-again quality.
+Redirect (•••): When you’re being attacked by multiple opponents, you can direct their blows against one another. When you Dodge, if your Defense roll reduces an attack’s successes to 0, your attacker rolls the same attack against another attacker of your choice.
+Drawback: You may only redirect one attack in a turn. You cannot redirect an attack against the same attacker.
+Joint Strike (••••): You wait until the last possible second then lash out at your opponent’s elbow or wrist as he attacks, hoping to cripple his limbs. Roll Strength + Brawl instead of Defense. If you score more successes than your attacker, you deal one point of bashing damage per extra success, and inflict either the Arm Wrack or Leg Wrack Tilt (your choice). Drawback: Spend a point of Willpower to use this maneuver.
+Like the Breeze (•••••): You step to one side as your opponent attacks and give her enough of a push to send her flying past you. When dodging, if your Defense roll reduces an opponent’s attack successes to 0, you can inflict the Knocked Down Tilt. Drawback: You must declare that you’re using this maneuver at the start of the turn before taking any other attacks.</t>
+  </si>
+  <si>
+    <t>You’re able to use a weapon to stop people who are trying to kill you. Often deployed by police officers using riot shields or ASP batons, it’s just as effective with a chair leg.
+Cover the Angles (•): Whenever you take a Dodge action, reduce the Defense penalties for multiple attackers by 1. You can apply your full Defense against the first two attacks, suffer a –1 penalty against the third, and so on.
+Weak Spot (••): You swing against your opponent’s arm rather than his own weapon. Use this ability when defendingagainst an armed attacker. If your Defense reduces his attack pool to 0, he’s disarmed. If you Dodge, you disarm your opponent if your Defense roll reduces his attack successes to 0.
+Aggressive Defense (•••): Anyone dumb enough to come near you is liable to get hurt. When you take a Dodge action, if you score more successes than any attacker, you deal one point of lethal damage to the attacker per extra success. Your weapon bonus doesn’t apply to this extra damage.
+Drawback: You must spend a point of Willpower and declare that you are using Aggressive Defense at the start of the turn. You cannot combine this maneuver with Press the Advantage or Weak Spot.
+Iron Guard (••••): You and your weapon are one. At the start of each turn, you can choose to reduce your weapon bonus (down to a minimum of 0) to increase your Defense by a like amount. If you take a Dodge action, add your full weapon bonus to your Defense after doubling your pool.
+Press the Advantage (•••••): You create an opening with a block and lash out with a fist or foot. When you’re taking a Dodge action, if your Defense roll reduces the attacker’s successes to 0, you can make an unarmed attack against that opponent at a −2 penalty. Your opponent applies Defense as normal. Drawback: Spend a point of Willpower to make the attack. You can only make one attack per turn in this way.</t>
+  </si>
+  <si>
+    <t>Close Quarters Combat (Style)</t>
+  </si>
+  <si>
+    <t>• to ••••</t>
   </si>
 </sst>
 </file>
@@ -1543,10 +1876,10 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1576,7 +1909,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="285" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" ht="342" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>72</v>
       </c>
@@ -1604,7 +1937,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="171" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>73</v>
       </c>
@@ -1656,7 +1989,7 @@
         <v>Your character cannot purchase the Fame Merit. This also may limit Status purchases, if the character cannot provide sufficient identification for the roles she wishes to take.</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>75</v>
       </c>
@@ -1681,7 +2014,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" ht="242.25" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>76</v>
       </c>
@@ -1734,7 +2067,7 @@
         <v>Any rolls to find or identify the character enjoy a +1 bonus per dot of the Merit. If the character has Alternate Identity, she can mitigate this drawback. A character with Fame cannot have the Anonymity Merit.</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="228" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" ht="256.5" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>78</v>
       </c>
@@ -1789,7 +2122,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="114" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>80</v>
       </c>
@@ -1814,7 +2147,7 @@
         <v>This Merit requires upkeep. You must attend at least monthly, informal meetings to maintain the benefits of Hobbyist Clique.</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="57" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>81</v>
       </c>
@@ -1865,7 +2198,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="228" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" ht="256.5" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>83</v>
       </c>
@@ -1892,7 +2225,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="270.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" ht="285" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>84</v>
       </c>
@@ -1925,7 +2258,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" ht="199.5" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>85</v>
       </c>
@@ -1977,7 +2310,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" ht="171" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>87</v>
       </c>
@@ -2005,7 +2338,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" ht="213.75" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>88</v>
       </c>
@@ -2057,7 +2390,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>90</v>
       </c>
@@ -2082,7 +2415,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" ht="313.5" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>91</v>
       </c>
@@ -2138,7 +2471,7 @@
         <v xml:space="preserve">Attention is a double-edged sword. Any rolls to spot, notice, or remember your character gain the same die bonus. Sometimes, your character will draw unwanted attention in social situations. This could cause further complications. </v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>93</v>
       </c>
@@ -2163,7 +2496,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="171" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" ht="185.25" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>94</v>
       </c>
@@ -2193,7 +2526,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" ht="99.75" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>95</v>
       </c>
@@ -2225,25 +2558,556 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0729954-66AC-4542-8D56-19E6506D5786}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48BA91AF-9DA8-4314-89CD-623615379EDE}">
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.86328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="77.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.73046875" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="299.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="A5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="142.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="156.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="142.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="356.25" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="242.25" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="142.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="285" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="156.75" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{093ECA82-A522-4AEE-97DF-9E38081AC98B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2551A4-BB1C-4096-8B17-C2793F928A93}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718E4D33-E789-4B04-A99C-68002B320071}">
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.53125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.9296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="126.3984375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="213.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="256.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A8" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="114" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="213.75" x14ac:dyDescent="0.45">
+      <c r="A10" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="313.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A12" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="242.25" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="213.75" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="256.5" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="213.75" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D19" xr:uid="{093ECA82-A522-4AEE-97DF-9E38081AC98B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout des Atouts de Lignagne (que j'avais oublié)
</commit_message>
<xml_diff>
--- a/Atouts.xlsx
+++ b/Atouts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bertolen\Documents\JdR\Univers\Chroniques des Ténèbres\Ferae\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X181880\OneDrive - GROUP DIGITAL WORKPLACE\Documents\Privé\Ferae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517BED78-E8F7-4AE6-980A-DFA478352E88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{517BED78-E8F7-4AE6-980A-DFA478352E88}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{32FE2937-FBA0-4115-B6D2-CB62A74651CC}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="28800" windowHeight="15435" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mentaux" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,13 @@
     <sheet name="Surnaturel (humain)" sheetId="7" r:id="rId4"/>
     <sheet name="Combat" sheetId="8" r:id="rId5"/>
     <sheet name="Uratha" sheetId="11" r:id="rId6"/>
-    <sheet name="Combat Uratha" sheetId="12" r:id="rId7"/>
+    <sheet name="Combat (Uratha)" sheetId="12" r:id="rId7"/>
+    <sheet name="Combat (Uratha) (2)" sheetId="15" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Combat!$A$1:$D$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Combat Uratha'!$A$1:$E$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Combat (Uratha)'!$A$1:$E$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Combat (Uratha) (2)'!$A$1:$E$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mentaux!$A$1:$E$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Physique!$A$1:$E$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sociaux!$A$1:$E$1</definedName>
@@ -38,9 +40,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="345">
   <si>
     <t>Nom</t>
   </si>
@@ -1201,6 +1201,66 @@
   </si>
   <si>
     <t>Parkour (Style)</t>
+  </si>
+  <si>
+    <t>BOND</t>
+  </si>
+  <si>
+    <t>• OR •••</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wolf-Blooded </t>
+  </si>
+  <si>
+    <t>Wolf-Blooded belong in packs, it’s a natural pull. However, how strongly they bond with the pack depends on their investment in serving the pack and the territory.
+Wolf-Blooded with one dot in this Merit are treated with the same level of respect as important Storyteller-character Wolf-Blooded, such as those created during Pack Creation (p. 90). They may purchase one dot of the Totem Merit and enjoy all the benefits of it.
+Wolf-Blooded characters with three dots in this Merit have proven themselves to the pack, or otherwise gain a natural respect from their Uratha cousins, and are a natural part of the hunting party. These respected and vital members of the pack can purchase up to five dots in the Totem Merit.</t>
+  </si>
+  <si>
+    <t>RAISED BY WOLVES</t>
+  </si>
+  <si>
+    <t>The character grew up in a pack, not an outsider alone and unaware of what he was. That sense of belonging went a long way to ease the character’s internal horror over what he was, but added a new level of stress. The Wolf-Blooded has an exact idea of what werewolves are, how dangerous the spirit world is, and how the mundane world is a lie. The Wolf-Blooded character does not need to succeed at Composure, Stamina, or Resolve rolls to withstand the mystical or biologically strange. This accounts for both physical and psychological responses.</t>
+  </si>
+  <si>
+    <t>TELL</t>
+  </si>
+  <si>
+    <t>The character develops a second Tell, chosen from those available to Wolf-Blooded. While the player chooses the new Tell, the character has no choice in how Father Luna or Mother Wolf’s touch develops.
+With Storyteller permission, a human character can buy this Merit with Experiences to represent a character who spontaneously becomes Wolf-Blooded.</t>
+  </si>
+  <si>
+    <t>CRESCENT MOON’S BIRTH</t>
+  </si>
+  <si>
+    <t>Wolf-Blooded born under the crescent moon with this Merit are the left hand of the fetish-crafter. Any fetish they’re involved in crafting gains +3 Durability and +3 Structure.</t>
+  </si>
+  <si>
+    <t>FULL MOON’S BIRTH</t>
+  </si>
+  <si>
+    <t>Without a full understanding of what it is to be a werewolf, full-moon-born Wolf-Blooded will never be the tacticians the Rahu are. And yet, a Wolf-Blooded with this Merit can manage and lead the rest of the pack in times when the Uratha are gone or otherwise occupied. Once per scene, when making a coordinated action that was planned in advance, spend a point of Willpower and an instant action. A number of characters equal to your character’s Presence can benefit from the +3 bonus from the Willpower expenditure, as well as the 8-again quality. Your character does not gain dice from Willpower as normal.</t>
+  </si>
+  <si>
+    <t>GIBBOUS MOON’S BIRTH</t>
+  </si>
+  <si>
+    <t>Those Wolf-Blooded born under the gibbous moon aren’t the natural lore masters that the Cahalith are, but they index and organize stories like the spirit of the Library of Alexandria. Select a Mental Skill. She gains 8-again on all rolls involving that Skill, and any extended actions with that Skill takes only half the normal amount of time.</t>
+  </si>
+  <si>
+    <t>HALF MOON’S BIRTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wolf-Blooded, Safe Place • </t>
+  </si>
+  <si>
+    <t>A Wolf-Blooded born under a half moon has a wide view of his pack and especially its territory. The wide view means that the territory is just a chess board for him, and his pack half the pieces. He gets +2 on all breaking point rolls when in his territory, and once per chapter he can choose to add his Safe Place dots and 8-again to a roll.</t>
+  </si>
+  <si>
+    <t>NO MOON’S BIRTH</t>
+  </si>
+  <si>
+    <t>Wolf-Blooded born under no moon are natural double agents. When out on a formal mission spying for his pack, any roll to detect where the no-moon came from or who sent her automatically fails. He carries no scent from his pack, and cannot be followed back to his home. The orders must be direct from a pack leader or specifically assigned by the Wolf-Blooded’s parental figure.</t>
   </si>
 </sst>
 </file>
@@ -1571,17 +1631,17 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.06640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="95.9296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="1" customWidth="1"/>
+    <col min="4" max="4" width="96" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.06640625" style="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1598,7 +1658,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1615,7 +1675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1632,7 +1692,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -1649,7 +1709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1666,7 +1726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
@@ -1683,7 +1743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -1700,7 +1760,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
@@ -1717,7 +1777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
@@ -1734,7 +1794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
@@ -1751,7 +1811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1768,7 +1828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>32</v>
       </c>
@@ -1785,7 +1845,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -1802,7 +1862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
@@ -1819,7 +1879,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
@@ -1836,7 +1896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="114" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>44</v>
       </c>
@@ -1853,7 +1913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>47</v>
       </c>
@@ -1870,7 +1930,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>49</v>
       </c>
@@ -1887,7 +1947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" ht="285" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>51</v>
       </c>
@@ -1904,7 +1964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>54</v>
       </c>
@@ -1921,7 +1981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>56</v>
       </c>
@@ -1949,23 +2009,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C862E33-7151-4155-B06F-70A6FA9AEF48}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" style="1"/>
-    <col min="4" max="4" width="87.796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.73046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1"/>
+    <col min="4" max="4" width="87.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1982,7 +2042,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>241</v>
       </c>
@@ -1999,7 +2059,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>243</v>
       </c>
@@ -2016,7 +2076,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>245</v>
       </c>
@@ -2033,7 +2093,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>247</v>
       </c>
@@ -2050,7 +2110,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>249</v>
       </c>
@@ -2067,7 +2127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>251</v>
       </c>
@@ -2084,7 +2144,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>253</v>
       </c>
@@ -2101,7 +2161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>255</v>
       </c>
@@ -2118,7 +2178,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="360" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>325</v>
       </c>
@@ -2135,7 +2195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>258</v>
       </c>
@@ -2152,7 +2212,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>260</v>
       </c>
@@ -2169,7 +2229,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>262</v>
       </c>
@@ -2203,16 +2263,16 @@
       <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.86328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="77.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.73046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="77.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2229,7 +2289,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="342" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="390" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>264</v>
       </c>
@@ -2246,7 +2306,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="171" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>266</v>
       </c>
@@ -2263,7 +2323,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>269</v>
       </c>
@@ -2280,7 +2340,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>272</v>
       </c>
@@ -2297,7 +2357,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="242.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>275</v>
       </c>
@@ -2314,7 +2374,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>277</v>
       </c>
@@ -2331,7 +2391,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="315" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>280</v>
       </c>
@@ -2348,7 +2408,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>282</v>
       </c>
@@ -2365,7 +2425,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>285</v>
       </c>
@@ -2382,7 +2442,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>289</v>
       </c>
@@ -2399,7 +2459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>292</v>
       </c>
@@ -2416,7 +2476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="285" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>295</v>
       </c>
@@ -2433,7 +2493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="285" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" ht="345" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>297</v>
       </c>
@@ -2450,7 +2510,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="199.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>299</v>
       </c>
@@ -2467,7 +2527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>301</v>
       </c>
@@ -2484,7 +2544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="171" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>304</v>
       </c>
@@ -2501,7 +2561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>306</v>
       </c>
@@ -2518,7 +2578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>308</v>
       </c>
@@ -2535,7 +2595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>310</v>
       </c>
@@ -2552,7 +2612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" ht="345" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>312</v>
       </c>
@@ -2569,7 +2629,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>315</v>
       </c>
@@ -2586,7 +2646,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>318</v>
       </c>
@@ -2603,7 +2663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>320</v>
       </c>
@@ -2620,7 +2680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>323</v>
       </c>
@@ -2654,16 +2714,16 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.86328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="77.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.73046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="77.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2680,7 +2740,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="299.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="345" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>60</v>
       </c>
@@ -2697,7 +2757,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
@@ -2714,7 +2774,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
@@ -2731,7 +2791,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>69</v>
       </c>
@@ -2748,7 +2808,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>71</v>
       </c>
@@ -2765,7 +2825,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>75</v>
       </c>
@@ -2782,7 +2842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>78</v>
       </c>
@@ -2799,7 +2859,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="356.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="405" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>81</v>
       </c>
@@ -2816,7 +2876,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="242.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="285" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>85</v>
       </c>
@@ -2833,7 +2893,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>88</v>
       </c>
@@ -2850,7 +2910,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="285" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="330" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>91</v>
       </c>
@@ -2867,7 +2927,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>94</v>
       </c>
@@ -2884,7 +2944,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>97</v>
       </c>
@@ -2918,15 +2978,15 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="126.3984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="126.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2940,7 +3000,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="270" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>99</v>
       </c>
@@ -2954,7 +3014,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>100</v>
       </c>
@@ -2968,7 +3028,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>102</v>
       </c>
@@ -2982,7 +3042,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="270" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>137</v>
       </c>
@@ -2996,7 +3056,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>104</v>
       </c>
@@ -3010,7 +3070,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>107</v>
       </c>
@@ -3024,7 +3084,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>109</v>
       </c>
@@ -3038,7 +3098,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="114" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>111</v>
       </c>
@@ -3052,7 +3112,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>113</v>
       </c>
@@ -3066,7 +3126,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" ht="360" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>115</v>
       </c>
@@ -3080,7 +3140,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>117</v>
       </c>
@@ -3094,7 +3154,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="242.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" ht="270" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>120</v>
       </c>
@@ -3108,7 +3168,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>122</v>
       </c>
@@ -3122,7 +3182,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>124</v>
       </c>
@@ -3136,7 +3196,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>126</v>
       </c>
@@ -3150,7 +3210,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>128</v>
       </c>
@@ -3164,7 +3224,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" ht="300" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>131</v>
       </c>
@@ -3178,7 +3238,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" ht="240" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>133</v>
       </c>
@@ -3209,16 +3269,16 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.86328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="77.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.73046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="77.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3235,7 +3295,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>139</v>
       </c>
@@ -3252,7 +3312,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>143</v>
       </c>
@@ -3269,7 +3329,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>147</v>
       </c>
@@ -3286,7 +3346,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>151</v>
       </c>
@@ -3303,7 +3363,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>154</v>
       </c>
@@ -3320,7 +3380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>156</v>
       </c>
@@ -3337,7 +3397,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>160</v>
       </c>
@@ -3354,7 +3414,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>164</v>
       </c>
@@ -3371,7 +3431,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>166</v>
       </c>
@@ -3388,7 +3448,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>169</v>
       </c>
@@ -3405,7 +3465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>172</v>
       </c>
@@ -3422,7 +3482,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>175</v>
       </c>
@@ -3439,7 +3499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>177</v>
       </c>
@@ -3456,7 +3516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>179</v>
       </c>
@@ -3473,7 +3533,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>182</v>
       </c>
@@ -3490,7 +3550,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>185</v>
       </c>
@@ -3507,7 +3567,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>189</v>
       </c>
@@ -3524,7 +3584,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>192</v>
       </c>
@@ -3541,7 +3601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>194</v>
       </c>
@@ -3558,7 +3618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>196</v>
       </c>
@@ -3575,7 +3635,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>198</v>
       </c>
@@ -3592,7 +3652,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>201</v>
       </c>
@@ -3609,7 +3669,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="114" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>204</v>
       </c>
@@ -3626,7 +3686,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="128.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>207</v>
       </c>
@@ -3658,19 +3718,19 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.86328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="77.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.73046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="77.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3687,7 +3747,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>211</v>
       </c>
@@ -3704,7 +3764,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>214</v>
       </c>
@@ -3721,7 +3781,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>217</v>
       </c>
@@ -3738,7 +3798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>219</v>
       </c>
@@ -3755,7 +3815,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="342" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="405" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>229</v>
       </c>
@@ -3772,7 +3832,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>222</v>
       </c>
@@ -3789,7 +3849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="342" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="405" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>230</v>
       </c>
@@ -3806,7 +3866,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>226</v>
       </c>
@@ -3821,6 +3881,185 @@
       </c>
       <c r="E9" s="5" t="s">
         <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E9" xr:uid="{093ECA82-A522-4AEE-97DF-9E38081AC98B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64FE8AB2-69D7-4663-A5FE-F885056643F8}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="77.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Avancement sur les Kitsune
</commit_message>
<xml_diff>
--- a/Atouts.xlsx
+++ b/Atouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X181880\OneDrive - GROUP DIGITAL WORKPLACE\Documents\Privé\Ferae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{517BED78-E8F7-4AE6-980A-DFA478352E88}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{32FE2937-FBA0-4115-B6D2-CB62A74651CC}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{517BED78-E8F7-4AE6-980A-DFA478352E88}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{BA0ED80F-140A-42FB-95B5-4FBA1D21C453}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="28800" windowHeight="15435" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mentaux" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,13 @@
     <sheet name="Combat" sheetId="8" r:id="rId5"/>
     <sheet name="Uratha" sheetId="11" r:id="rId6"/>
     <sheet name="Combat (Uratha)" sheetId="12" r:id="rId7"/>
-    <sheet name="Combat (Uratha) (2)" sheetId="15" r:id="rId8"/>
+    <sheet name="Parent (Uratha)" sheetId="15" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Combat!$A$1:$D$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Combat (Uratha)'!$A$1:$E$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Combat (Uratha) (2)'!$A$1:$E$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mentaux!$A$1:$E$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Parent (Uratha)'!$A$1:$E$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Physique!$A$1:$E$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sociaux!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Surnaturel (humain)'!$A$1:$E$1</definedName>
@@ -934,9 +934,6 @@
     <t>Giant</t>
   </si>
   <si>
-    <t>haracter is massive. She’s well over six feet tall and crowds part when she approaches. She’s Size 6 and gains +1 Health. Available only at character creation.</t>
-  </si>
-  <si>
     <t>Hardy</t>
   </si>
   <si>
@@ -970,9 +967,6 @@
   </si>
   <si>
     <t>Small-Framed</t>
-  </si>
-  <si>
-    <t>haracter is diminutive. She’s not even five feet tall and it’s easy to walk into her without noticing. She’s Size 4 and thus has one fewer Health box. She gains +2 to any rolls to hide or go unnoticed. This bonus might apply any time being smaller would be an advantage, such as crawling through smaller spaces. Available only at character creation.</t>
   </si>
   <si>
     <t>Allie</t>
@@ -1261,6 +1255,12 @@
   </si>
   <si>
     <t>Wolf-Blooded born under no moon are natural double agents. When out on a formal mission spying for his pack, any roll to detect where the no-moon came from or who sent her automatically fails. He carries no scent from his pack, and cannot be followed back to his home. The orders must be direct from a pack leader or specifically assigned by the Wolf-Blooded’s parental figure.</t>
+  </si>
+  <si>
+    <t>Your character is massive. She’s well over six feet tall and crowds part when she approaches. She’s Size 6 and gains +1 Health. Available only at character creation.</t>
+  </si>
+  <si>
+    <t>Your character is diminutive. She’s not even five feet tall and it’s easy to walk into her without noticing. She’s Size 4 and thus has one fewer Health box. She gains +2 to any rolls to hide or go unnoticed. This bonus might apply any time being smaller would be an advantage, such as crawling through smaller spaces. Available only at character creation.</t>
   </si>
 </sst>
 </file>
@@ -2009,16 +2009,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C862E33-7151-4155-B06F-70A6FA9AEF48}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="1"/>
     <col min="4" max="4" width="87.85546875" style="1" customWidth="1"/>
@@ -2138,7 +2138,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>252</v>
+        <v>343</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>231</v>
@@ -2146,7 +2146,7 @@
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>42</v>
@@ -2155,7 +2155,7 @@
         <v>239</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>7</v>
@@ -2163,7 +2163,7 @@
     </row>
     <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>42</v>
@@ -2172,7 +2172,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>7</v>
@@ -2180,7 +2180,7 @@
     </row>
     <row r="10" spans="1:5" ht="360" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>52</v>
@@ -2189,7 +2189,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>7</v>
@@ -2197,7 +2197,7 @@
     </row>
     <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>26</v>
@@ -2206,7 +2206,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>7</v>
@@ -2214,7 +2214,7 @@
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>33</v>
@@ -2223,7 +2223,7 @@
         <v>238</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>7</v>
@@ -2231,7 +2231,7 @@
     </row>
     <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>33</v>
@@ -2240,7 +2240,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>263</v>
+        <v>344</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>232</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="2" spans="1:5" ht="390" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>52</v>
@@ -2300,7 +2300,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>7</v>
@@ -2308,16 +2308,16 @@
     </row>
     <row r="3" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>268</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>7</v>
@@ -2325,7 +2325,7 @@
     </row>
     <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>52</v>
@@ -2334,24 +2334,24 @@
         <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>7</v>
@@ -2359,7 +2359,7 @@
     </row>
     <row r="6" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>52</v>
@@ -2368,7 +2368,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>7</v>
@@ -2376,7 +2376,7 @@
     </row>
     <row r="7" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>42</v>
@@ -2385,15 +2385,15 @@
         <v>7</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="315" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>233</v>
@@ -2402,7 +2402,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>7</v>
@@ -2410,16 +2410,16 @@
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>7</v>
@@ -2427,33 +2427,33 @@
     </row>
     <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>286</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>7</v>
@@ -2461,16 +2461,16 @@
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>7</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="13" spans="1:5" ht="285" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>52</v>
@@ -2487,7 +2487,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>7</v>
@@ -2495,7 +2495,7 @@
     </row>
     <row r="14" spans="1:5" ht="345" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>52</v>
@@ -2504,7 +2504,7 @@
         <v>7</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>7</v>
@@ -2512,7 +2512,7 @@
     </row>
     <row r="15" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>52</v>
@@ -2521,7 +2521,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>7</v>
@@ -2529,16 +2529,16 @@
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>7</v>
@@ -2546,7 +2546,7 @@
     </row>
     <row r="17" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>52</v>
@@ -2555,7 +2555,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>7</v>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="18" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>52</v>
@@ -2572,7 +2572,7 @@
         <v>7</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>7</v>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>33</v>
@@ -2589,7 +2589,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>7</v>
@@ -2597,7 +2597,7 @@
     </row>
     <row r="20" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>52</v>
@@ -2606,7 +2606,7 @@
         <v>7</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>7</v>
@@ -2614,7 +2614,7 @@
     </row>
     <row r="21" spans="1:5" ht="345" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>52</v>
@@ -2623,15 +2623,15 @@
         <v>7</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>129</v>
@@ -2640,15 +2640,15 @@
         <v>7</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>33</v>
@@ -2657,7 +2657,7 @@
         <v>7</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>7</v>
@@ -2665,16 +2665,16 @@
     </row>
     <row r="24" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>7</v>
@@ -2682,7 +2682,7 @@
     </row>
     <row r="25" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>61</v>
@@ -2691,7 +2691,7 @@
         <v>7</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>7</v>
@@ -3893,11 +3893,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64FE8AB2-69D7-4663-A5FE-F885056643F8}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3928,16 +3928,16 @@
     </row>
     <row r="2" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>327</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>329</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>7</v>
@@ -3945,16 +3945,16 @@
     </row>
     <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>7</v>
@@ -3962,16 +3962,16 @@
     </row>
     <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>61</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>7</v>
@@ -3979,16 +3979,16 @@
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>7</v>
@@ -3996,16 +3996,16 @@
     </row>
     <row r="6" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>7</v>
@@ -4013,16 +4013,16 @@
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>7</v>
@@ -4030,16 +4030,16 @@
     </row>
     <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>7</v>
@@ -4047,16 +4047,16 @@
     </row>
     <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>7</v>

</xml_diff>